<commit_message>
Change the variable from leftstr to righstr id from iffound==0
</commit_message>
<xml_diff>
--- a/Python/Split Address Regex/Split Address.xlsx
+++ b/Python/Split Address Regex/Split Address.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jimmy Yang\OneDrive\Work Portfolio\Python\Split Address Regex\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jimmy Yang\OneDrive\Work Portfolio\Personal Projects\Programming\Python\Split Address Regex\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2" documentId="11_8F44074C9B0032EF9968E71E0CFB798E780B7473" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{49DA3ABE-B04E-42B0-8659-1990FDEF766E}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="11_8F441D44F2B1F4C46EF5E67D0AB779CC515570A5" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{0B5E324D-979E-4335-9DF4-3EDC74799E28}"/>
   <bookViews>
-    <workbookView xWindow="-20" yWindow="60" windowWidth="22610" windowHeight="21050" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2560" yWindow="3370" windowWidth="28800" windowHeight="15610" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="226" uniqueCount="147">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="114">
   <si>
     <t>Customer ID</t>
   </si>
@@ -62,18 +62,9 @@
     <t>Croydon</t>
   </si>
   <si>
-    <t xml:space="preserve">Building ABC </t>
-  </si>
-  <si>
     <t>Unit 32</t>
   </si>
   <si>
-    <t>15</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Hay </t>
-  </si>
-  <si>
     <t>Street</t>
   </si>
   <si>
@@ -89,12 +80,6 @@
     <t>Sydney</t>
   </si>
   <si>
-    <t>10</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Bay </t>
-  </si>
-  <si>
     <t>Ave</t>
   </si>
   <si>
@@ -107,9 +92,6 @@
     <t>Manly</t>
   </si>
   <si>
-    <t xml:space="preserve"> Market </t>
-  </si>
-  <si>
     <t>Road</t>
   </si>
   <si>
@@ -122,18 +104,6 @@
     <t>123/ 11-15 Hunter Lane</t>
   </si>
   <si>
-    <t xml:space="preserve">Broadway Plaza </t>
-  </si>
-  <si>
-    <t xml:space="preserve">123 </t>
-  </si>
-  <si>
-    <t>11-15</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Hunter </t>
-  </si>
-  <si>
     <t>Lane</t>
   </si>
   <si>
@@ -146,15 +116,6 @@
     <t>Parramatta</t>
   </si>
   <si>
-    <t xml:space="preserve">EEE Villeage </t>
-  </si>
-  <si>
-    <t>5</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Second </t>
-  </si>
-  <si>
     <t>Customer 6</t>
   </si>
   <si>
@@ -164,12 +125,6 @@
     <t>Burwood</t>
   </si>
   <si>
-    <t>11 - 14</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Main </t>
-  </si>
-  <si>
     <t>Customer 7</t>
   </si>
   <si>
@@ -179,15 +134,6 @@
     <t>Ashfield</t>
   </si>
   <si>
-    <t>U32</t>
-  </si>
-  <si>
-    <t>90</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> View </t>
-  </si>
-  <si>
     <t>Drive</t>
   </si>
   <si>
@@ -200,15 +146,6 @@
     <t>Surry Hill</t>
   </si>
   <si>
-    <t>No 45</t>
-  </si>
-  <si>
-    <t>300</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Lake </t>
-  </si>
-  <si>
     <t>Customer 9</t>
   </si>
   <si>
@@ -218,39 +155,18 @@
     <t>38 Fourth Avenue</t>
   </si>
   <si>
-    <t>38</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Fourth </t>
-  </si>
-  <si>
-    <t>Avenue</t>
-  </si>
-  <si>
     <t>Customer 10</t>
   </si>
   <si>
     <t>40 Cooper Road</t>
   </si>
   <si>
-    <t>40</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Cooper </t>
-  </si>
-  <si>
     <t>Customer 11</t>
   </si>
   <si>
     <t>100 Sydney Highway</t>
   </si>
   <si>
-    <t>100</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Sydney </t>
-  </si>
-  <si>
     <t>Highway</t>
   </si>
   <si>
@@ -263,15 +179,6 @@
     <t>St Peter</t>
   </si>
   <si>
-    <t xml:space="preserve">35A </t>
-  </si>
-  <si>
-    <t>150</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> St Peter </t>
-  </si>
-  <si>
     <t>Customer 13</t>
   </si>
   <si>
@@ -281,12 +188,6 @@
     <t>Summer Hill</t>
   </si>
   <si>
-    <t>2</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Queens </t>
-  </si>
-  <si>
     <t>Customer 14</t>
   </si>
   <si>
@@ -296,12 +197,6 @@
     <t>Strathfield</t>
   </si>
   <si>
-    <t>50</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Wellington </t>
-  </si>
-  <si>
     <t>Place</t>
   </si>
   <si>
@@ -317,13 +212,19 @@
     <t>Blacktown</t>
   </si>
   <si>
-    <t xml:space="preserve">Garden Building </t>
-  </si>
-  <si>
-    <t>Unit 785</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> ABC </t>
+    <t>Customer 16</t>
+  </si>
+  <si>
+    <t>Unit 31 A 53 BCH Street</t>
+  </si>
+  <si>
+    <t>Wollongong</t>
+  </si>
+  <si>
+    <t>Customer 17</t>
+  </si>
+  <si>
+    <t>Unit 11 Abert Building 52 Abert Street</t>
   </si>
   <si>
     <t>All Type</t>
@@ -841,22 +742,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J16"/>
+  <dimension ref="A1:J18"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="H20" sqref="H20"/>
+      <selection activeCell="F2" sqref="F2:J18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="11.1796875" style="4" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.36328125" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.453125" style="4" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="31" style="4" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="20.7265625" style="4" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.90625" style="4" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.6328125" style="4" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.08984375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.08984375" style="4" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.81640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.54296875" style="4" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.1796875" style="4" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.1796875" style="4" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="10.1796875" style="4" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -905,402 +806,310 @@
       <c r="E2" t="s">
         <v>12</v>
       </c>
-      <c r="F2" t="s">
-        <v>13</v>
-      </c>
-      <c r="G2" t="s">
-        <v>14</v>
-      </c>
-      <c r="H2" t="s">
-        <v>15</v>
-      </c>
-      <c r="I2" t="s">
-        <v>16</v>
-      </c>
-      <c r="J2" t="s">
-        <v>17</v>
-      </c>
+      <c r="F2"/>
+      <c r="G2"/>
+      <c r="I2"/>
+      <c r="J2"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>112</v>
       </c>
       <c r="B3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E3" t="s">
         <v>18</v>
       </c>
-      <c r="C3" t="s">
-        <v>19</v>
-      </c>
-      <c r="D3" t="s">
-        <v>20</v>
-      </c>
-      <c r="E3" t="s">
-        <v>21</v>
-      </c>
       <c r="F3"/>
-      <c r="G3" t="s">
-        <v>19</v>
-      </c>
-      <c r="H3" t="s">
-        <v>22</v>
-      </c>
-      <c r="I3" t="s">
-        <v>23</v>
-      </c>
-      <c r="J3" t="s">
-        <v>24</v>
-      </c>
+      <c r="G3"/>
+      <c r="I3"/>
+      <c r="J3"/>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>113</v>
       </c>
       <c r="B4" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="C4" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="E4" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="F4"/>
-      <c r="H4" t="s">
-        <v>22</v>
-      </c>
-      <c r="I4" t="s">
-        <v>28</v>
-      </c>
-      <c r="J4" t="s">
-        <v>29</v>
-      </c>
+      <c r="G4"/>
+      <c r="I4"/>
+      <c r="J4"/>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>114</v>
       </c>
       <c r="B5" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="C5" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="D5" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="E5" t="s">
-        <v>21</v>
-      </c>
-      <c r="F5" t="s">
-        <v>33</v>
-      </c>
-      <c r="G5" t="s">
-        <v>34</v>
-      </c>
-      <c r="H5" t="s">
-        <v>35</v>
-      </c>
-      <c r="I5" t="s">
-        <v>36</v>
-      </c>
-      <c r="J5" t="s">
-        <v>37</v>
-      </c>
+        <v>18</v>
+      </c>
+      <c r="F5"/>
+      <c r="G5"/>
+      <c r="I5"/>
+      <c r="J5"/>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>115</v>
       </c>
       <c r="B6" t="s">
-        <v>38</v>
+        <v>28</v>
       </c>
       <c r="C6" t="s">
-        <v>39</v>
+        <v>29</v>
       </c>
       <c r="E6" t="s">
-        <v>40</v>
-      </c>
-      <c r="F6" t="s">
-        <v>41</v>
-      </c>
-      <c r="H6" t="s">
-        <v>42</v>
-      </c>
-      <c r="I6" t="s">
-        <v>43</v>
-      </c>
-      <c r="J6" t="s">
-        <v>29</v>
-      </c>
+        <v>30</v>
+      </c>
+      <c r="F6"/>
+      <c r="G6"/>
+      <c r="I6"/>
+      <c r="J6"/>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>116</v>
       </c>
       <c r="B7" t="s">
-        <v>44</v>
+        <v>31</v>
       </c>
       <c r="C7" t="s">
-        <v>45</v>
+        <v>32</v>
       </c>
       <c r="E7" t="s">
-        <v>46</v>
+        <v>33</v>
       </c>
       <c r="F7"/>
-      <c r="H7" t="s">
-        <v>47</v>
-      </c>
-      <c r="I7" t="s">
-        <v>48</v>
-      </c>
-      <c r="J7" t="s">
-        <v>29</v>
-      </c>
+      <c r="G7"/>
+      <c r="I7"/>
+      <c r="J7"/>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>117</v>
       </c>
       <c r="B8" t="s">
-        <v>49</v>
+        <v>34</v>
       </c>
       <c r="C8" t="s">
-        <v>50</v>
+        <v>35</v>
       </c>
       <c r="E8" t="s">
-        <v>51</v>
+        <v>36</v>
       </c>
       <c r="F8"/>
-      <c r="G8" t="s">
-        <v>52</v>
-      </c>
-      <c r="H8" t="s">
-        <v>53</v>
-      </c>
-      <c r="I8" t="s">
-        <v>54</v>
-      </c>
-      <c r="J8" t="s">
-        <v>55</v>
-      </c>
+      <c r="G8"/>
+      <c r="I8"/>
+      <c r="J8"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>118</v>
       </c>
       <c r="B9" t="s">
-        <v>56</v>
+        <v>38</v>
       </c>
       <c r="C9" t="s">
-        <v>57</v>
+        <v>39</v>
       </c>
       <c r="E9" t="s">
-        <v>58</v>
+        <v>40</v>
       </c>
       <c r="F9"/>
-      <c r="G9" t="s">
-        <v>59</v>
-      </c>
-      <c r="H9" t="s">
-        <v>60</v>
-      </c>
-      <c r="I9" t="s">
-        <v>61</v>
-      </c>
-      <c r="J9" t="s">
-        <v>29</v>
-      </c>
+      <c r="G9"/>
+      <c r="I9"/>
+      <c r="J9"/>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>119</v>
       </c>
       <c r="B10" t="s">
-        <v>62</v>
+        <v>41</v>
       </c>
       <c r="C10" t="s">
-        <v>63</v>
+        <v>42</v>
       </c>
       <c r="D10" t="s">
-        <v>64</v>
+        <v>43</v>
       </c>
       <c r="E10" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="F10"/>
-      <c r="G10" t="s">
-        <v>63</v>
-      </c>
-      <c r="H10" t="s">
-        <v>65</v>
-      </c>
-      <c r="I10" t="s">
-        <v>66</v>
-      </c>
-      <c r="J10" t="s">
-        <v>67</v>
-      </c>
+      <c r="G10"/>
+      <c r="I10"/>
+      <c r="J10"/>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>120</v>
       </c>
       <c r="B11" t="s">
-        <v>68</v>
+        <v>44</v>
       </c>
       <c r="C11" t="s">
-        <v>69</v>
+        <v>45</v>
       </c>
       <c r="E11" t="s">
-        <v>46</v>
+        <v>33</v>
       </c>
       <c r="F11"/>
-      <c r="H11" t="s">
-        <v>70</v>
-      </c>
-      <c r="I11" t="s">
-        <v>71</v>
-      </c>
-      <c r="J11" t="s">
-        <v>29</v>
-      </c>
+      <c r="G11"/>
+      <c r="I11"/>
+      <c r="J11"/>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>121</v>
       </c>
       <c r="B12" t="s">
-        <v>72</v>
+        <v>46</v>
       </c>
       <c r="C12" t="s">
-        <v>73</v>
+        <v>47</v>
       </c>
       <c r="E12" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="F12"/>
-      <c r="H12" t="s">
-        <v>74</v>
-      </c>
-      <c r="I12" t="s">
-        <v>75</v>
-      </c>
-      <c r="J12" t="s">
-        <v>76</v>
-      </c>
+      <c r="G12"/>
+      <c r="I12"/>
+      <c r="J12"/>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>122</v>
       </c>
       <c r="B13" t="s">
-        <v>77</v>
+        <v>49</v>
       </c>
       <c r="C13" t="s">
-        <v>78</v>
+        <v>50</v>
       </c>
       <c r="E13" t="s">
-        <v>79</v>
+        <v>51</v>
       </c>
       <c r="F13"/>
-      <c r="G13" t="s">
-        <v>80</v>
-      </c>
-      <c r="H13" t="s">
-        <v>81</v>
-      </c>
-      <c r="I13" t="s">
-        <v>82</v>
-      </c>
-      <c r="J13" t="s">
-        <v>24</v>
-      </c>
+      <c r="G13"/>
+      <c r="I13"/>
+      <c r="J13"/>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>123</v>
       </c>
       <c r="B14" t="s">
-        <v>83</v>
+        <v>52</v>
       </c>
       <c r="D14" t="s">
-        <v>84</v>
+        <v>53</v>
       </c>
       <c r="E14" t="s">
-        <v>85</v>
+        <v>54</v>
       </c>
       <c r="F14"/>
-      <c r="H14" t="s">
-        <v>86</v>
-      </c>
-      <c r="I14" t="s">
-        <v>87</v>
-      </c>
-      <c r="J14" t="s">
-        <v>17</v>
-      </c>
+      <c r="G14"/>
+      <c r="I14"/>
+      <c r="J14"/>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>124</v>
       </c>
       <c r="B15" t="s">
-        <v>88</v>
+        <v>55</v>
       </c>
       <c r="C15" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D15" t="s">
-        <v>89</v>
+        <v>56</v>
       </c>
       <c r="E15" t="s">
-        <v>90</v>
+        <v>57</v>
       </c>
       <c r="F15"/>
-      <c r="G15" t="s">
-        <v>14</v>
-      </c>
-      <c r="H15" t="s">
-        <v>91</v>
-      </c>
-      <c r="I15" t="s">
-        <v>92</v>
-      </c>
-      <c r="J15" t="s">
-        <v>93</v>
-      </c>
+      <c r="G15"/>
+      <c r="I15"/>
+      <c r="J15"/>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>125</v>
       </c>
       <c r="B16" t="s">
-        <v>94</v>
+        <v>59</v>
       </c>
       <c r="C16" t="s">
-        <v>95</v>
+        <v>60</v>
       </c>
       <c r="D16" t="s">
-        <v>96</v>
+        <v>61</v>
       </c>
       <c r="E16" t="s">
-        <v>97</v>
-      </c>
-      <c r="F16" t="s">
-        <v>98</v>
-      </c>
-      <c r="G16" t="s">
-        <v>99</v>
-      </c>
-      <c r="H16" t="s">
-        <v>15</v>
-      </c>
-      <c r="I16" t="s">
-        <v>100</v>
-      </c>
-      <c r="J16" t="s">
-        <v>29</v>
-      </c>
+        <v>62</v>
+      </c>
+      <c r="F16"/>
+      <c r="G16"/>
+      <c r="I16"/>
+      <c r="J16"/>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A17">
+        <v>126</v>
+      </c>
+      <c r="B17" t="s">
+        <v>63</v>
+      </c>
+      <c r="C17" t="s">
+        <v>64</v>
+      </c>
+      <c r="E17" t="s">
+        <v>65</v>
+      </c>
+      <c r="F17"/>
+      <c r="G17"/>
+      <c r="I17"/>
+      <c r="J17"/>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A18">
+        <v>127</v>
+      </c>
+      <c r="B18" t="s">
+        <v>66</v>
+      </c>
+      <c r="C18" t="s">
+        <v>67</v>
+      </c>
+      <c r="F18"/>
+      <c r="G18"/>
+      <c r="I18"/>
+      <c r="J18"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1318,436 +1127,436 @@
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="9.453125" style="4" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.08984375" style="4" customWidth="1"/>
+    <col min="3" max="3" width="11.1796875" style="4" customWidth="1"/>
     <col min="4" max="4" width="11.54296875" style="4" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
-        <v>101</v>
+        <v>68</v>
       </c>
       <c r="C1" s="3" t="s">
         <v>9</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>102</v>
+        <v>69</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="C2" t="s">
-        <v>103</v>
+        <v>70</v>
       </c>
       <c r="D2" t="s">
-        <v>104</v>
+        <v>71</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="C3" t="s">
-        <v>105</v>
+        <v>72</v>
       </c>
       <c r="D3" t="s">
-        <v>106</v>
+        <v>73</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>107</v>
+        <v>74</v>
       </c>
       <c r="C4" t="s">
-        <v>108</v>
+        <v>75</v>
       </c>
       <c r="D4" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>109</v>
+        <v>76</v>
       </c>
       <c r="C5" t="s">
-        <v>110</v>
+        <v>77</v>
       </c>
       <c r="D5" t="s">
-        <v>111</v>
+        <v>78</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>108</v>
+        <v>75</v>
       </c>
       <c r="C6" t="s">
-        <v>112</v>
+        <v>79</v>
       </c>
       <c r="D6" t="s">
-        <v>113</v>
+        <v>80</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="C7" t="s">
-        <v>114</v>
+        <v>81</v>
       </c>
       <c r="D7" t="s">
-        <v>115</v>
+        <v>82</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>37</v>
+        <v>27</v>
       </c>
       <c r="C8" t="s">
-        <v>116</v>
+        <v>83</v>
       </c>
       <c r="D8" t="s">
-        <v>117</v>
+        <v>84</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>55</v>
+        <v>37</v>
       </c>
       <c r="C9" t="s">
-        <v>118</v>
+        <v>85</v>
       </c>
       <c r="D9" t="s">
-        <v>119</v>
+        <v>86</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>76</v>
+        <v>48</v>
       </c>
       <c r="C10" t="s">
-        <v>120</v>
+        <v>87</v>
       </c>
       <c r="D10" t="s">
-        <v>121</v>
+        <v>88</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>93</v>
+        <v>58</v>
       </c>
       <c r="C11" t="s">
-        <v>122</v>
+        <v>89</v>
       </c>
       <c r="D11" t="s">
-        <v>123</v>
+        <v>90</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>123</v>
+        <v>90</v>
       </c>
       <c r="C12" t="s">
-        <v>124</v>
+        <v>91</v>
       </c>
       <c r="D12" t="s">
-        <v>125</v>
+        <v>92</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>103</v>
+        <v>70</v>
       </c>
       <c r="C13" t="s">
-        <v>55</v>
+        <v>37</v>
       </c>
       <c r="D13" t="s">
-        <v>126</v>
+        <v>93</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>126</v>
+        <v>93</v>
       </c>
       <c r="C14" t="s">
-        <v>127</v>
+        <v>94</v>
       </c>
       <c r="D14" t="s">
-        <v>128</v>
+        <v>95</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>129</v>
+        <v>96</v>
       </c>
       <c r="C15" t="s">
-        <v>130</v>
+        <v>97</v>
       </c>
       <c r="D15" t="s">
-        <v>131</v>
+        <v>98</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>105</v>
+        <v>72</v>
       </c>
       <c r="C16" t="s">
-        <v>132</v>
+        <v>99</v>
       </c>
       <c r="D16" t="s">
-        <v>133</v>
+        <v>100</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>122</v>
+        <v>89</v>
       </c>
       <c r="C17" t="s">
-        <v>76</v>
+        <v>48</v>
       </c>
       <c r="D17" t="s">
-        <v>129</v>
+        <v>96</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>110</v>
+        <v>77</v>
       </c>
       <c r="C18" t="s">
-        <v>134</v>
+        <v>101</v>
       </c>
       <c r="D18" t="s">
-        <v>135</v>
+        <v>102</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>112</v>
+        <v>79</v>
       </c>
       <c r="C19" t="s">
-        <v>37</v>
+        <v>27</v>
       </c>
       <c r="D19" t="s">
-        <v>37</v>
+        <v>27</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
-        <v>114</v>
+        <v>81</v>
       </c>
       <c r="C20" t="s">
-        <v>136</v>
+        <v>103</v>
       </c>
       <c r="D20" t="s">
-        <v>136</v>
+        <v>103</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
-        <v>116</v>
+        <v>83</v>
       </c>
       <c r="C21" t="s">
-        <v>137</v>
+        <v>104</v>
       </c>
       <c r="D21" t="s">
-        <v>137</v>
+        <v>104</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
-        <v>120</v>
+        <v>87</v>
       </c>
       <c r="C22" t="s">
-        <v>138</v>
+        <v>105</v>
       </c>
       <c r="D22" t="s">
-        <v>139</v>
+        <v>106</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
-        <v>124</v>
+        <v>91</v>
       </c>
       <c r="C23" t="s">
-        <v>93</v>
+        <v>58</v>
       </c>
       <c r="D23" t="s">
-        <v>140</v>
+        <v>107</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
-        <v>127</v>
+        <v>94</v>
       </c>
       <c r="C24" t="s">
-        <v>141</v>
+        <v>108</v>
       </c>
       <c r="D24" t="s">
-        <v>142</v>
+        <v>109</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
-        <v>130</v>
+        <v>97</v>
       </c>
       <c r="C25" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="D25" t="s">
-        <v>109</v>
+        <v>76</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
-        <v>132</v>
+        <v>99</v>
       </c>
       <c r="C26" t="s">
-        <v>143</v>
+        <v>110</v>
       </c>
       <c r="D26" t="s">
-        <v>144</v>
+        <v>111</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
-        <v>118</v>
+        <v>85</v>
       </c>
       <c r="C27" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="D27" t="s">
-        <v>107</v>
+        <v>74</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
-        <v>134</v>
+        <v>101</v>
       </c>
       <c r="C28" t="s">
-        <v>145</v>
+        <v>112</v>
       </c>
       <c r="D28" t="s">
-        <v>146</v>
+        <v>113</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
-        <v>138</v>
+        <v>105</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
-        <v>141</v>
+        <v>108</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
-        <v>143</v>
+        <v>110</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
-        <v>145</v>
+        <v>112</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
-        <v>104</v>
+        <v>71</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
-        <v>106</v>
+        <v>73</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
-        <v>111</v>
+        <v>78</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
-        <v>113</v>
+        <v>80</v>
       </c>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
-        <v>115</v>
+        <v>82</v>
       </c>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
-        <v>117</v>
+        <v>84</v>
       </c>
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
-        <v>119</v>
+        <v>86</v>
       </c>
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
-        <v>121</v>
+        <v>88</v>
       </c>
     </row>
     <row r="41" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
-        <v>125</v>
+        <v>92</v>
       </c>
     </row>
     <row r="42" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
-        <v>128</v>
+        <v>95</v>
       </c>
     </row>
     <row r="43" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
-        <v>131</v>
+        <v>98</v>
       </c>
     </row>
     <row r="44" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
-        <v>133</v>
+        <v>100</v>
       </c>
     </row>
     <row r="45" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
-        <v>135</v>
+        <v>102</v>
       </c>
     </row>
     <row r="46" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
-        <v>136</v>
+        <v>103</v>
       </c>
     </row>
     <row r="47" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
-        <v>137</v>
+        <v>104</v>
       </c>
     </row>
     <row r="48" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
-        <v>139</v>
+        <v>106</v>
       </c>
     </row>
     <row r="49" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
-        <v>140</v>
+        <v>107</v>
       </c>
     </row>
     <row r="50" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
-        <v>142</v>
+        <v>109</v>
       </c>
     </row>
     <row r="51" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
-        <v>144</v>
+        <v>111</v>
       </c>
     </row>
     <row r="52" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
-        <v>146</v>
+        <v>113</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add strip to remove white space
</commit_message>
<xml_diff>
--- a/Python/Split Address Regex/Split Address.xlsx
+++ b/Python/Split Address Regex/Split Address.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jimmy Yang\OneDrive\Work Portfolio\Personal Projects\Programming\Python\Split Address Regex\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/581effd24fbd6252/Work Portfolio/Personal Projects - Github/Programming/Python/Split Address Regex/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="11_8F441D44F2B1F4C46EF5E67D0AB779CC515570A5" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{0B5E324D-979E-4335-9DF4-3EDC74799E28}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="11_4C43223C41D7A6A71FF4331A195E6398DE3E1112" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2560" yWindow="3370" windowWidth="28800" windowHeight="15610" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6555" yWindow="150" windowWidth="21600" windowHeight="15225" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="156">
   <si>
     <t>Customer ID</t>
   </si>
@@ -62,9 +62,18 @@
     <t>Croydon</t>
   </si>
   <si>
+    <t xml:space="preserve">Building ABC </t>
+  </si>
+  <si>
     <t>Unit 32</t>
   </si>
   <si>
+    <t>15</t>
+  </si>
+  <si>
+    <t>Hay</t>
+  </si>
+  <si>
     <t>Street</t>
   </si>
   <si>
@@ -80,6 +89,12 @@
     <t>Sydney</t>
   </si>
   <si>
+    <t>10</t>
+  </si>
+  <si>
+    <t>Bay</t>
+  </si>
+  <si>
     <t>Ave</t>
   </si>
   <si>
@@ -92,6 +107,9 @@
     <t>Manly</t>
   </si>
   <si>
+    <t>Market</t>
+  </si>
+  <si>
     <t>Road</t>
   </si>
   <si>
@@ -104,6 +122,15 @@
     <t>123/ 11-15 Hunter Lane</t>
   </si>
   <si>
+    <t>123</t>
+  </si>
+  <si>
+    <t>11-15</t>
+  </si>
+  <si>
+    <t>Hunter</t>
+  </si>
+  <si>
     <t>Lane</t>
   </si>
   <si>
@@ -116,6 +143,15 @@
     <t>Parramatta</t>
   </si>
   <si>
+    <t xml:space="preserve">EEE Villeage </t>
+  </si>
+  <si>
+    <t>5</t>
+  </si>
+  <si>
+    <t>Second</t>
+  </si>
+  <si>
     <t>Customer 6</t>
   </si>
   <si>
@@ -125,6 +161,12 @@
     <t>Burwood</t>
   </si>
   <si>
+    <t>11 - 14</t>
+  </si>
+  <si>
+    <t>Main</t>
+  </si>
+  <si>
     <t>Customer 7</t>
   </si>
   <si>
@@ -134,6 +176,15 @@
     <t>Ashfield</t>
   </si>
   <si>
+    <t>U32</t>
+  </si>
+  <si>
+    <t>90</t>
+  </si>
+  <si>
+    <t>View</t>
+  </si>
+  <si>
     <t>Drive</t>
   </si>
   <si>
@@ -146,6 +197,15 @@
     <t>Surry Hill</t>
   </si>
   <si>
+    <t>No 45</t>
+  </si>
+  <si>
+    <t>300</t>
+  </si>
+  <si>
+    <t>Lake</t>
+  </si>
+  <si>
     <t>Customer 9</t>
   </si>
   <si>
@@ -155,18 +215,36 @@
     <t>38 Fourth Avenue</t>
   </si>
   <si>
+    <t>38</t>
+  </si>
+  <si>
+    <t>Fourth</t>
+  </si>
+  <si>
+    <t>Avenue</t>
+  </si>
+  <si>
     <t>Customer 10</t>
   </si>
   <si>
     <t>40 Cooper Road</t>
   </si>
   <si>
+    <t>40</t>
+  </si>
+  <si>
+    <t>Cooper</t>
+  </si>
+  <si>
     <t>Customer 11</t>
   </si>
   <si>
     <t>100 Sydney Highway</t>
   </si>
   <si>
+    <t>100</t>
+  </si>
+  <si>
     <t>Highway</t>
   </si>
   <si>
@@ -179,6 +257,12 @@
     <t>St Peter</t>
   </si>
   <si>
+    <t>35A</t>
+  </si>
+  <si>
+    <t>150</t>
+  </si>
+  <si>
     <t>Customer 13</t>
   </si>
   <si>
@@ -188,6 +272,12 @@
     <t>Summer Hill</t>
   </si>
   <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>Queens</t>
+  </si>
+  <si>
     <t>Customer 14</t>
   </si>
   <si>
@@ -197,6 +287,12 @@
     <t>Strathfield</t>
   </si>
   <si>
+    <t>50</t>
+  </si>
+  <si>
+    <t>Wellington</t>
+  </si>
+  <si>
     <t>Place</t>
   </si>
   <si>
@@ -212,6 +308,15 @@
     <t>Blacktown</t>
   </si>
   <si>
+    <t xml:space="preserve">Garden Building </t>
+  </si>
+  <si>
+    <t>Unit 785</t>
+  </si>
+  <si>
+    <t>ABC</t>
+  </si>
+  <si>
     <t>Customer 16</t>
   </si>
   <si>
@@ -221,10 +326,31 @@
     <t>Wollongong</t>
   </si>
   <si>
+    <t>Unit 31 A</t>
+  </si>
+  <si>
+    <t>53</t>
+  </si>
+  <si>
+    <t>BCH</t>
+  </si>
+  <si>
     <t>Customer 17</t>
   </si>
   <si>
     <t>Unit 11 Abert Building 52 Abert Street</t>
+  </si>
+  <si>
+    <t>Abert Building</t>
+  </si>
+  <si>
+    <t>Unit 11</t>
+  </si>
+  <si>
+    <t>52</t>
+  </si>
+  <si>
+    <t>Abert</t>
   </si>
   <si>
     <t>All Type</t>
@@ -745,23 +871,23 @@
   <dimension ref="A1:J18"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2:J18"/>
+      <selection activeCell="I18" sqref="I18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.1796875" style="4" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.453125" style="4" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.140625" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.42578125" style="4" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="31" style="4" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="20.7265625" style="4" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.81640625" style="4" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.54296875" style="4" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.1796875" style="4" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.1796875" style="4" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.1796875" style="4" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.7109375" style="4" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.85546875" style="4" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.5703125" style="4" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.140625" style="4" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.140625" style="4" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.140625" style="4" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -793,7 +919,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>111</v>
       </c>
@@ -806,310 +932,461 @@
       <c r="E2" t="s">
         <v>12</v>
       </c>
-      <c r="F2"/>
-      <c r="G2"/>
-      <c r="I2"/>
-      <c r="J2"/>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="F2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G2" t="s">
+        <v>14</v>
+      </c>
+      <c r="H2" t="s">
+        <v>15</v>
+      </c>
+      <c r="I2" t="s">
+        <v>16</v>
+      </c>
+      <c r="J2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>112</v>
       </c>
       <c r="B3" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="C3" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="D3" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="E3" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="F3"/>
-      <c r="G3"/>
-      <c r="I3"/>
-      <c r="J3"/>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="G3" t="s">
+        <v>19</v>
+      </c>
+      <c r="H3" t="s">
+        <v>22</v>
+      </c>
+      <c r="I3" t="s">
+        <v>23</v>
+      </c>
+      <c r="J3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>113</v>
       </c>
       <c r="B4" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="C4" t="s">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="E4" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="F4"/>
       <c r="G4"/>
-      <c r="I4"/>
-      <c r="J4"/>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="H4" t="s">
+        <v>22</v>
+      </c>
+      <c r="I4" t="s">
+        <v>28</v>
+      </c>
+      <c r="J4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>114</v>
       </c>
       <c r="B5" t="s">
-        <v>24</v>
+        <v>30</v>
       </c>
       <c r="C5" t="s">
-        <v>25</v>
+        <v>31</v>
       </c>
       <c r="D5" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="E5" t="s">
-        <v>18</v>
-      </c>
-      <c r="F5"/>
-      <c r="G5"/>
-      <c r="I5"/>
-      <c r="J5"/>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
+        <v>21</v>
+      </c>
+      <c r="F5" t="s">
+        <v>31</v>
+      </c>
+      <c r="G5" t="s">
+        <v>33</v>
+      </c>
+      <c r="H5" t="s">
+        <v>34</v>
+      </c>
+      <c r="I5" t="s">
+        <v>35</v>
+      </c>
+      <c r="J5" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>115</v>
       </c>
       <c r="B6" t="s">
-        <v>28</v>
+        <v>37</v>
       </c>
       <c r="C6" t="s">
+        <v>38</v>
+      </c>
+      <c r="E6" t="s">
+        <v>39</v>
+      </c>
+      <c r="F6" t="s">
+        <v>40</v>
+      </c>
+      <c r="G6"/>
+      <c r="H6" t="s">
+        <v>41</v>
+      </c>
+      <c r="I6" t="s">
+        <v>42</v>
+      </c>
+      <c r="J6" t="s">
         <v>29</v>
       </c>
-      <c r="E6" t="s">
-        <v>30</v>
-      </c>
-      <c r="F6"/>
-      <c r="G6"/>
-      <c r="I6"/>
-      <c r="J6"/>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>116</v>
       </c>
       <c r="B7" t="s">
-        <v>31</v>
+        <v>43</v>
       </c>
       <c r="C7" t="s">
-        <v>32</v>
+        <v>44</v>
       </c>
       <c r="E7" t="s">
-        <v>33</v>
+        <v>45</v>
       </c>
       <c r="F7"/>
       <c r="G7"/>
-      <c r="I7"/>
-      <c r="J7"/>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="H7" t="s">
+        <v>46</v>
+      </c>
+      <c r="I7" t="s">
+        <v>47</v>
+      </c>
+      <c r="J7" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>117</v>
       </c>
       <c r="B8" t="s">
-        <v>34</v>
+        <v>48</v>
       </c>
       <c r="C8" t="s">
-        <v>35</v>
+        <v>49</v>
       </c>
       <c r="E8" t="s">
-        <v>36</v>
+        <v>50</v>
       </c>
       <c r="F8"/>
-      <c r="G8"/>
-      <c r="I8"/>
-      <c r="J8"/>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="G8" t="s">
+        <v>51</v>
+      </c>
+      <c r="H8" t="s">
+        <v>52</v>
+      </c>
+      <c r="I8" t="s">
+        <v>53</v>
+      </c>
+      <c r="J8" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>118</v>
       </c>
       <c r="B9" t="s">
-        <v>38</v>
+        <v>55</v>
       </c>
       <c r="C9" t="s">
-        <v>39</v>
+        <v>56</v>
       </c>
       <c r="E9" t="s">
-        <v>40</v>
+        <v>57</v>
       </c>
       <c r="F9"/>
-      <c r="G9"/>
-      <c r="I9"/>
-      <c r="J9"/>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="G9" t="s">
+        <v>58</v>
+      </c>
+      <c r="H9" t="s">
+        <v>59</v>
+      </c>
+      <c r="I9" t="s">
+        <v>60</v>
+      </c>
+      <c r="J9" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>119</v>
       </c>
       <c r="B10" t="s">
-        <v>41</v>
+        <v>61</v>
       </c>
       <c r="C10" t="s">
-        <v>42</v>
+        <v>62</v>
       </c>
       <c r="D10" t="s">
-        <v>43</v>
+        <v>63</v>
       </c>
       <c r="E10" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="F10"/>
-      <c r="G10"/>
-      <c r="I10"/>
-      <c r="J10"/>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="G10" t="s">
+        <v>62</v>
+      </c>
+      <c r="H10" t="s">
+        <v>64</v>
+      </c>
+      <c r="I10" t="s">
+        <v>65</v>
+      </c>
+      <c r="J10" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>120</v>
       </c>
       <c r="B11" t="s">
-        <v>44</v>
+        <v>67</v>
       </c>
       <c r="C11" t="s">
+        <v>68</v>
+      </c>
+      <c r="E11" t="s">
         <v>45</v>
-      </c>
-      <c r="E11" t="s">
-        <v>33</v>
       </c>
       <c r="F11"/>
       <c r="G11"/>
-      <c r="I11"/>
-      <c r="J11"/>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="H11" t="s">
+        <v>69</v>
+      </c>
+      <c r="I11" t="s">
+        <v>70</v>
+      </c>
+      <c r="J11" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>121</v>
       </c>
       <c r="B12" t="s">
-        <v>46</v>
+        <v>71</v>
       </c>
       <c r="C12" t="s">
-        <v>47</v>
+        <v>72</v>
       </c>
       <c r="E12" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="F12"/>
       <c r="G12"/>
-      <c r="I12"/>
-      <c r="J12"/>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="H12" t="s">
+        <v>73</v>
+      </c>
+      <c r="I12" t="s">
+        <v>21</v>
+      </c>
+      <c r="J12" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>122</v>
       </c>
       <c r="B13" t="s">
-        <v>49</v>
+        <v>75</v>
       </c>
       <c r="C13" t="s">
-        <v>50</v>
+        <v>76</v>
       </c>
       <c r="E13" t="s">
-        <v>51</v>
+        <v>77</v>
       </c>
       <c r="F13"/>
-      <c r="G13"/>
-      <c r="I13"/>
-      <c r="J13"/>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="G13" t="s">
+        <v>78</v>
+      </c>
+      <c r="H13" t="s">
+        <v>79</v>
+      </c>
+      <c r="I13" t="s">
+        <v>77</v>
+      </c>
+      <c r="J13" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>123</v>
       </c>
       <c r="B14" t="s">
-        <v>52</v>
+        <v>80</v>
       </c>
       <c r="D14" t="s">
-        <v>53</v>
+        <v>81</v>
       </c>
       <c r="E14" t="s">
-        <v>54</v>
+        <v>82</v>
       </c>
       <c r="F14"/>
       <c r="G14"/>
-      <c r="I14"/>
-      <c r="J14"/>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="H14" t="s">
+        <v>83</v>
+      </c>
+      <c r="I14" t="s">
+        <v>84</v>
+      </c>
+      <c r="J14" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>124</v>
       </c>
       <c r="B15" t="s">
-        <v>55</v>
+        <v>85</v>
       </c>
       <c r="C15" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D15" t="s">
-        <v>56</v>
+        <v>86</v>
       </c>
       <c r="E15" t="s">
-        <v>57</v>
+        <v>87</v>
       </c>
       <c r="F15"/>
-      <c r="G15"/>
-      <c r="I15"/>
-      <c r="J15"/>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="G15" t="s">
+        <v>14</v>
+      </c>
+      <c r="H15" t="s">
+        <v>88</v>
+      </c>
+      <c r="I15" t="s">
+        <v>89</v>
+      </c>
+      <c r="J15" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>125</v>
       </c>
       <c r="B16" t="s">
-        <v>59</v>
+        <v>91</v>
       </c>
       <c r="C16" t="s">
-        <v>60</v>
+        <v>92</v>
       </c>
       <c r="D16" t="s">
-        <v>61</v>
+        <v>93</v>
       </c>
       <c r="E16" t="s">
-        <v>62</v>
-      </c>
-      <c r="F16"/>
-      <c r="G16"/>
-      <c r="I16"/>
-      <c r="J16"/>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.35">
+        <v>94</v>
+      </c>
+      <c r="F16" t="s">
+        <v>95</v>
+      </c>
+      <c r="G16" t="s">
+        <v>96</v>
+      </c>
+      <c r="H16" t="s">
+        <v>15</v>
+      </c>
+      <c r="I16" t="s">
+        <v>97</v>
+      </c>
+      <c r="J16" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>126</v>
       </c>
       <c r="B17" t="s">
-        <v>63</v>
+        <v>98</v>
       </c>
       <c r="C17" t="s">
-        <v>64</v>
+        <v>99</v>
       </c>
       <c r="E17" t="s">
-        <v>65</v>
+        <v>100</v>
       </c>
       <c r="F17"/>
-      <c r="G17"/>
-      <c r="I17"/>
-      <c r="J17"/>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="G17" t="s">
+        <v>101</v>
+      </c>
+      <c r="H17" t="s">
+        <v>102</v>
+      </c>
+      <c r="I17" t="s">
+        <v>103</v>
+      </c>
+      <c r="J17" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>127</v>
       </c>
       <c r="B18" t="s">
-        <v>66</v>
+        <v>104</v>
       </c>
       <c r="C18" t="s">
-        <v>67</v>
-      </c>
-      <c r="F18"/>
-      <c r="G18"/>
-      <c r="I18"/>
-      <c r="J18"/>
+        <v>105</v>
+      </c>
+      <c r="F18" t="s">
+        <v>106</v>
+      </c>
+      <c r="G18" t="s">
+        <v>107</v>
+      </c>
+      <c r="H18" t="s">
+        <v>108</v>
+      </c>
+      <c r="I18" t="s">
+        <v>109</v>
+      </c>
+      <c r="J18" t="s">
+        <v>17</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1124,439 +1401,439 @@
       <selection activeCell="E21" sqref="E20:E21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.453125" style="4" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.1796875" style="4" customWidth="1"/>
-    <col min="4" max="4" width="11.54296875" style="4" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.42578125" style="4" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.140625" style="4" customWidth="1"/>
+    <col min="4" max="4" width="11.5703125" style="4" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>68</v>
+        <v>110</v>
       </c>
       <c r="C1" s="3" t="s">
         <v>9</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="C2" t="s">
-        <v>70</v>
+        <v>112</v>
       </c>
       <c r="D2" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
       <c r="C3" t="s">
-        <v>72</v>
+        <v>114</v>
       </c>
       <c r="D3" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>116</v>
+      </c>
+      <c r="C4" t="s">
+        <v>117</v>
+      </c>
+      <c r="D4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>118</v>
+      </c>
+      <c r="C5" t="s">
+        <v>119</v>
+      </c>
+      <c r="D5" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>117</v>
+      </c>
+      <c r="C6" t="s">
+        <v>121</v>
+      </c>
+      <c r="D6" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>24</v>
+      </c>
+      <c r="C7" t="s">
+        <v>123</v>
+      </c>
+      <c r="D7" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>36</v>
+      </c>
+      <c r="C8" t="s">
+        <v>125</v>
+      </c>
+      <c r="D8" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>54</v>
+      </c>
+      <c r="C9" t="s">
+        <v>127</v>
+      </c>
+      <c r="D9" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
         <v>74</v>
       </c>
-      <c r="C4" t="s">
-        <v>75</v>
-      </c>
-      <c r="D4" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
-        <v>76</v>
-      </c>
-      <c r="C5" t="s">
-        <v>77</v>
-      </c>
-      <c r="D5" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A6" t="s">
-        <v>75</v>
-      </c>
-      <c r="C6" t="s">
-        <v>79</v>
-      </c>
-      <c r="D6" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A7" t="s">
-        <v>19</v>
-      </c>
-      <c r="C7" t="s">
-        <v>81</v>
-      </c>
-      <c r="D7" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A8" t="s">
-        <v>27</v>
-      </c>
-      <c r="C8" t="s">
-        <v>83</v>
-      </c>
-      <c r="D8" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A9" t="s">
-        <v>37</v>
-      </c>
-      <c r="C9" t="s">
-        <v>85</v>
-      </c>
-      <c r="D9" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A10" t="s">
-        <v>48</v>
-      </c>
       <c r="C10" t="s">
-        <v>87</v>
+        <v>129</v>
       </c>
       <c r="D10" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>58</v>
+        <v>90</v>
       </c>
       <c r="C11" t="s">
-        <v>89</v>
+        <v>131</v>
       </c>
       <c r="D11" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>132</v>
+      </c>
+      <c r="C12" t="s">
+        <v>133</v>
+      </c>
+      <c r="D12" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>112</v>
+      </c>
+      <c r="C13" t="s">
+        <v>54</v>
+      </c>
+      <c r="D13" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>135</v>
+      </c>
+      <c r="C14" t="s">
+        <v>136</v>
+      </c>
+      <c r="D14" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>138</v>
+      </c>
+      <c r="C15" t="s">
+        <v>139</v>
+      </c>
+      <c r="D15" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>114</v>
+      </c>
+      <c r="C16" t="s">
+        <v>141</v>
+      </c>
+      <c r="D16" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>131</v>
+      </c>
+      <c r="C17" t="s">
+        <v>74</v>
+      </c>
+      <c r="D17" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>119</v>
+      </c>
+      <c r="C18" t="s">
+        <v>143</v>
+      </c>
+      <c r="D18" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>121</v>
+      </c>
+      <c r="C19" t="s">
+        <v>36</v>
+      </c>
+      <c r="D19" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>123</v>
+      </c>
+      <c r="C20" t="s">
+        <v>145</v>
+      </c>
+      <c r="D20" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>125</v>
+      </c>
+      <c r="C21" t="s">
+        <v>146</v>
+      </c>
+      <c r="D21" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>129</v>
+      </c>
+      <c r="C22" t="s">
+        <v>147</v>
+      </c>
+      <c r="D22" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>133</v>
+      </c>
+      <c r="C23" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A12" t="s">
-        <v>90</v>
-      </c>
-      <c r="C12" t="s">
-        <v>91</v>
-      </c>
-      <c r="D12" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A13" t="s">
-        <v>70</v>
-      </c>
-      <c r="C13" t="s">
-        <v>37</v>
-      </c>
-      <c r="D13" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A14" t="s">
-        <v>93</v>
-      </c>
-      <c r="C14" t="s">
-        <v>94</v>
-      </c>
-      <c r="D14" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A15" t="s">
-        <v>96</v>
-      </c>
-      <c r="C15" t="s">
-        <v>97</v>
-      </c>
-      <c r="D15" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A16" t="s">
-        <v>72</v>
-      </c>
-      <c r="C16" t="s">
-        <v>99</v>
-      </c>
-      <c r="D16" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A17" t="s">
-        <v>89</v>
-      </c>
-      <c r="C17" t="s">
-        <v>48</v>
-      </c>
-      <c r="D17" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A18" t="s">
-        <v>77</v>
-      </c>
-      <c r="C18" t="s">
-        <v>101</v>
-      </c>
-      <c r="D18" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A19" t="s">
-        <v>79</v>
-      </c>
-      <c r="C19" t="s">
-        <v>27</v>
-      </c>
-      <c r="D19" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A20" t="s">
-        <v>81</v>
-      </c>
-      <c r="C20" t="s">
-        <v>103</v>
-      </c>
-      <c r="D20" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A21" t="s">
-        <v>83</v>
-      </c>
-      <c r="C21" t="s">
-        <v>104</v>
-      </c>
-      <c r="D21" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A22" t="s">
-        <v>87</v>
-      </c>
-      <c r="C22" t="s">
-        <v>105</v>
-      </c>
-      <c r="D22" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A23" t="s">
-        <v>91</v>
-      </c>
-      <c r="C23" t="s">
-        <v>58</v>
-      </c>
       <c r="D23" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.35">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>94</v>
+        <v>136</v>
       </c>
       <c r="C24" t="s">
-        <v>108</v>
+        <v>150</v>
       </c>
       <c r="D24" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.35">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>97</v>
+        <v>139</v>
       </c>
       <c r="C25" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
       <c r="D25" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.35">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>99</v>
+        <v>141</v>
       </c>
       <c r="C26" t="s">
-        <v>110</v>
+        <v>152</v>
       </c>
       <c r="D26" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.35">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>85</v>
+        <v>127</v>
       </c>
       <c r="C27" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="D27" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.35">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>101</v>
+        <v>143</v>
       </c>
       <c r="C28" t="s">
-        <v>112</v>
+        <v>154</v>
       </c>
       <c r="D28" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A29" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A30" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A31" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A32" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A33" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.35">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.35">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.35">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.35">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.35">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.35">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.35">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.35">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.35">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.35">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.35">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.35">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.35">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.35">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.35">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.35">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.35">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.35">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>113</v>
+        <v>155</v>
       </c>
     </row>
   </sheetData>

</xml_diff>